<commit_message>
correciones de reporte mensual de 50
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/CalculoFacturaCpgnaConFee50.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/CalculoFacturaCpgnaConFee50.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414229C4-C5DA-475C-B6C8-C94453CC88CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F9FF3C-0615-4AAF-9307-F0C1AD1E746E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="701" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fact CPGNA" sheetId="2" r:id="rId1"/>
-    <sheet name="factura" sheetId="7" state="hidden" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="8" r:id="rId2"/>
+    <sheet name="factura" sheetId="7" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="\A">#REF!</definedName>
@@ -31,10 +32,11 @@
     <definedName name="\V">#REF!</definedName>
     <definedName name="\W">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Fact CPGNA'!$B$2:$K$93</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">factura!$E$10:$L$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">factura!$E$10:$L$53</definedName>
     <definedName name="AREPORTE_DIARI">#REF!</definedName>
     <definedName name="AREPORTE1">#REF!</definedName>
     <definedName name="BALANCE1">#REF!</definedName>
+    <definedName name="BarrilesProducto_Items">Hoja1!$L$8:$Q$9</definedName>
     <definedName name="GASEST">#REF!</definedName>
     <definedName name="MARCIANITO">#REF!</definedName>
     <definedName name="MARCIANITO20">#REF!</definedName>
@@ -45,6 +47,7 @@
     <definedName name="reporte">#REF!</definedName>
     <definedName name="REPORTE_DIARIO">#REF!</definedName>
     <definedName name="REPORTE1">#REF!</definedName>
+    <definedName name="ResumenEntrega_Items">Hoja1!$B$8:$I$9</definedName>
     <definedName name="TipoCambio_Items">'Fact CPGNA'!$I$9:$J$10</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
   <si>
     <r>
       <t xml:space="preserve">A) Determinación del </t>
@@ -755,6 +758,120 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>BOLETA DEL PROMEDIO MENSUAL VOLUMEN DE PROCESAMIENTO GAS NATURAL ASOCIADO (GNA)</t>
+  </si>
+  <si>
+    <t>BOLETA MENSUAL DEL VOLUMEN TOTAL PRODUCIDO DE CPGNA, GLP Y CGN</t>
+  </si>
+  <si>
+    <t>MES:</t>
+  </si>
+  <si>
+    <t>Volumen</t>
+  </si>
+  <si>
+    <t>Horas no procesadas</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>CPGNA (*)</t>
+  </si>
+  <si>
+    <t>GLP</t>
+  </si>
+  <si>
+    <t>CGN</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>CNPC</t>
+  </si>
+  <si>
+    <t>No procesado</t>
+  </si>
+  <si>
+    <t>Planta F/S</t>
+  </si>
+  <si>
+    <t>Ajuste con Plantas E/S</t>
+  </si>
+  <si>
+    <t>Procesado</t>
+  </si>
+  <si>
+    <t>Barriles</t>
+  </si>
+  <si>
+    <t>Número de días del período mensual =</t>
+  </si>
+  <si>
+    <t>días</t>
+  </si>
+  <si>
+    <t>(*) CPGNA: Componentes Pesados del Gas Natural Asociado.</t>
+  </si>
+  <si>
+    <t>MMPCD</t>
+  </si>
+  <si>
+    <t>UNNA ENERGIA S.A</t>
+  </si>
+  <si>
+    <t>ENEL Generación Piura S.A</t>
+  </si>
+  <si>
+    <t>{{item.Fecha}}</t>
+  </si>
+  <si>
+    <t>{{item.Cnpc}}</t>
+  </si>
+  <si>
+    <t>{{item.Total}}</t>
+  </si>
+  <si>
+    <t>{{item.NoProcesado}}</t>
+  </si>
+  <si>
+    <t>{{item.PlantaFs}}</t>
+  </si>
+  <si>
+    <t>{{item.AjustePlantaFs}}</t>
+  </si>
+  <si>
+    <t>{{item.Procesado}}</t>
+  </si>
+  <si>
+    <t>{{item.ProcesadoHoras}}</t>
+  </si>
+  <si>
+    <t>{{NumeroDiasPeriodo}}</t>
+  </si>
+  <si>
+    <t>{{Mmpcd}}</t>
+  </si>
+  <si>
+    <t>{{CentajeTotal}}</t>
+  </si>
+  <si>
+    <t>{{CentajeCgn}}</t>
+  </si>
+  <si>
+    <t>{{CentajeGlp}}</t>
+  </si>
+  <si>
+    <t>{{item.Cgn}}</t>
+  </si>
+  <si>
+    <t>{{item.Glp}}</t>
+  </si>
 </sst>
 </file>
 
@@ -779,7 +896,7 @@
     <numFmt numFmtId="179" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     <numFmt numFmtId="180" formatCode="[$-280A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
-  <fonts count="73">
+  <fonts count="76">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1255,6 +1372,25 @@
       <color indexed="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1468,7 +1604,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1819,8 +1955,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="357">
+  <cellStyleXfs count="358">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="173" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2187,8 +2334,9 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2471,6 +2619,74 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="357" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="125" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="125"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="357" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="47" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2483,21 +2699,35 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="357">
+  <cellStyles count="358">
     <cellStyle name="20% - Énfasis1" xfId="52" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis1 2" xfId="161" xr:uid="{BC31B0FA-7ECA-42A2-BF2F-58BC3EDDF6B7}"/>
     <cellStyle name="20% - Énfasis1 3" xfId="196" xr:uid="{EBD5C74F-BAFF-41BB-B203-6B292FE296B1}"/>
@@ -2832,6 +3062,7 @@
     <cellStyle name="Normal 9 6 4" xfId="299" xr:uid="{B622046E-61BA-42DC-ADEE-4638FE476886}"/>
     <cellStyle name="Normal 9 6 5" xfId="333" xr:uid="{CDCCFAE6-0AD5-4D43-BDFA-B4BA143500F4}"/>
     <cellStyle name="Normal 9 7" xfId="152" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal_Boleta diaria GMP-EEPSA" xfId="357" xr:uid="{5154C9AC-AEE3-47F7-AF26-E49221A996C8}"/>
     <cellStyle name="Normal_NÚM_ EN LETRAS_REV1" xfId="32" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
     <cellStyle name="Notas 2" xfId="158" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
     <cellStyle name="Notas 2 2" xfId="193" xr:uid="{E7280A75-27F0-4B8A-8DFD-D98312633A50}"/>
@@ -2856,7 +3087,18 @@
     <cellStyle name="Título 4" xfId="159" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
     <cellStyle name="Total" xfId="50" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2971,6 +3213,129 @@
         <a:xfrm>
           <a:off x="5921096" y="268605"/>
           <a:ext cx="928316" cy="395312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>112374</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60430</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="112374" y="85724"/>
+          <a:ext cx="1068725" cy="460481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171905</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>73817</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>356114</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7544255" y="73817"/>
+          <a:ext cx="946209" cy="402932"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3345,7 +3710,7 @@
   </sheetPr>
   <dimension ref="B2:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="145" zoomScaleNormal="85" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="145" zoomScaleNormal="85" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -3365,23 +3730,23 @@
       <c r="N2" s="90"/>
     </row>
     <row r="3" spans="3:18">
-      <c r="C3" s="135" t="s">
+      <c r="C3" s="171" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
       <c r="N3" s="88"/>
     </row>
     <row r="4" spans="3:18">
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135"/>
-      <c r="H4" s="135"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
       <c r="N4" s="89"/>
     </row>
     <row r="5" spans="3:18">
@@ -3405,19 +3770,19 @@
     </row>
     <row r="8" spans="3:18" ht="12.75" customHeight="1">
       <c r="G8" s="91"/>
-      <c r="I8" s="136" t="s">
+      <c r="I8" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="137"/>
+      <c r="J8" s="173"/>
       <c r="M8" s="82"/>
       <c r="N8" s="7"/>
       <c r="O8" s="83"/>
     </row>
     <row r="9" spans="3:18" ht="13.5" customHeight="1">
-      <c r="C9" s="134" t="s">
+      <c r="C9" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="134"/>
+      <c r="D9" s="170"/>
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
@@ -3769,42 +4134,42 @@
       <c r="R31" s="55"/>
     </row>
     <row r="32" spans="3:18">
-      <c r="C32" s="140" t="s">
+      <c r="C32" s="174" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="140"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="140"/>
-      <c r="G32" s="140"/>
-      <c r="H32" s="140"/>
-      <c r="I32" s="141"/>
-      <c r="J32" s="141"/>
+      <c r="D32" s="174"/>
+      <c r="E32" s="174"/>
+      <c r="F32" s="174"/>
+      <c r="G32" s="174"/>
+      <c r="H32" s="174"/>
+      <c r="I32" s="135"/>
+      <c r="J32" s="135"/>
       <c r="M32" s="62"/>
       <c r="N32" s="54"/>
       <c r="O32" s="54"/>
       <c r="P32" s="55"/>
     </row>
     <row r="33" spans="3:12">
-      <c r="C33" s="142" t="s">
+      <c r="C33" s="169" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="142"/>
-      <c r="E33" s="142"/>
-      <c r="F33" s="142"/>
-      <c r="G33" s="142"/>
-      <c r="H33" s="142"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="169"/>
+      <c r="F33" s="169"/>
+      <c r="G33" s="169"/>
+      <c r="H33" s="169"/>
       <c r="I33" s="84"/>
       <c r="J33" s="84"/>
     </row>
     <row r="34" spans="3:12">
-      <c r="C34" s="142" t="s">
+      <c r="C34" s="169" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="142"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="142"/>
-      <c r="H34" s="142"/>
+      <c r="D34" s="169"/>
+      <c r="E34" s="169"/>
+      <c r="F34" s="169"/>
+      <c r="G34" s="169"/>
+      <c r="H34" s="169"/>
       <c r="I34" s="84"/>
       <c r="J34" s="84"/>
     </row>
@@ -4214,6 +4579,307 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C20844-8914-4D92-B039-BDC0FF141079}">
+  <dimension ref="B2:R24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="2" spans="2:18">
+      <c r="C2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="2:18" ht="15.75">
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="M3" s="137"/>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="N4" s="134" t="s">
+        <v>164</v>
+      </c>
+      <c r="O4" s="138"/>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="139" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="177" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="178"/>
+      <c r="H6" s="140" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="140" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="M6" s="142" t="s">
+        <v>168</v>
+      </c>
+      <c r="O6" s="140" t="s">
+        <v>169</v>
+      </c>
+      <c r="P6" s="140" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q6" s="140" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="22.5">
+      <c r="B7" s="140" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="143" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="140" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="140" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="140" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="144" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="140" t="s">
+        <v>177</v>
+      </c>
+      <c r="I7" s="140" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="140" t="s">
+        <v>172</v>
+      </c>
+      <c r="M7" s="145" t="s">
+        <v>178</v>
+      </c>
+      <c r="N7" s="141"/>
+      <c r="O7" s="140" t="s">
+        <v>178</v>
+      </c>
+      <c r="P7" s="140" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q7" s="140" t="s">
+        <v>178</v>
+      </c>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="146" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="147" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="148" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="148" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="149" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="149" t="s">
+        <v>190</v>
+      </c>
+      <c r="H8" s="148" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="150" t="s">
+        <v>192</v>
+      </c>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="146" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="N8" s="13"/>
+      <c r="O8" s="149" t="s">
+        <v>199</v>
+      </c>
+      <c r="P8" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q8" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="146"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="166"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="150"/>
+      <c r="J9" s="141"/>
+      <c r="K9" s="141"/>
+      <c r="L9" s="146"/>
+      <c r="M9" s="149"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="151"/>
+      <c r="P9" s="151"/>
+      <c r="Q9" s="151"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="L10" s="153"/>
+      <c r="M10" s="154"/>
+      <c r="N10" s="152"/>
+      <c r="O10" s="155" t="s">
+        <v>197</v>
+      </c>
+      <c r="P10" s="155" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q10" s="155" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="153"/>
+      <c r="D11" s="154" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="167" t="s">
+        <v>193</v>
+      </c>
+      <c r="I11" t="s">
+        <v>180</v>
+      </c>
+      <c r="L11" s="153"/>
+      <c r="M11" s="154"/>
+      <c r="N11" s="152"/>
+      <c r="O11" s="154"/>
+      <c r="P11" s="154"/>
+      <c r="Q11" s="154"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="153"/>
+      <c r="C12" s="154"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="154"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
+      <c r="L12" s="156" t="s">
+        <v>181</v>
+      </c>
+      <c r="M12" s="154"/>
+      <c r="N12" s="152"/>
+      <c r="O12" s="154"/>
+      <c r="Q12" s="154"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="C13" s="154"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="168" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" s="159" t="s">
+        <v>182</v>
+      </c>
+      <c r="M13" s="154"/>
+      <c r="N13" s="152"/>
+      <c r="O13" s="154"/>
+      <c r="P13" s="160"/>
+      <c r="Q13" s="154"/>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="C21" s="107"/>
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161"/>
+      <c r="J21" s="163"/>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="C22" s="175" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="175"/>
+      <c r="E22" s="175"/>
+      <c r="G22" s="175" t="s">
+        <v>184</v>
+      </c>
+      <c r="H22" s="175"/>
+      <c r="I22" s="175"/>
+      <c r="J22" s="164"/>
+      <c r="K22" s="182"/>
+      <c r="L22" s="181" t="s">
+        <v>183</v>
+      </c>
+      <c r="M22" s="175"/>
+      <c r="O22" s="175" t="s">
+        <v>184</v>
+      </c>
+      <c r="P22" s="175"/>
+      <c r="Q22" s="175"/>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="B24" s="162"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="L22:M22"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N8:N9">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C6:U134"/>
   <sheetViews>
@@ -4274,10 +4940,10 @@
     </row>
     <row r="16" spans="4:11" ht="25.5" customHeight="1"/>
     <row r="17" spans="5:15" ht="27" customHeight="1">
-      <c r="J17" s="138" t="s">
+      <c r="J17" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="138"/>
+      <c r="K17" s="179"/>
       <c r="L17" s="24" t="s">
         <v>68</v>
       </c>
@@ -4301,11 +4967,11 @@
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="139" t="str">
+      <c r="J19" s="180" t="str">
         <f>+'Fact CPGNA'!E68</f>
         <v>{{CmPrecioPsec}}</v>
       </c>
-      <c r="K19" s="139"/>
+      <c r="K19" s="180"/>
       <c r="L19" s="99" t="e">
         <f>ROUND(+E19*J19,2)</f>
         <v>#VALUE!</v>
@@ -4327,8 +4993,8 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="139"/>
-      <c r="K21" s="139"/>
+      <c r="J21" s="180"/>
+      <c r="K21" s="180"/>
       <c r="L21" s="99"/>
     </row>
     <row r="22" spans="5:15">
@@ -4411,8 +5077,8 @@
       <c r="G29" s="34"/>
       <c r="H29" s="35"/>
       <c r="I29" s="36"/>
-      <c r="J29" s="138"/>
-      <c r="K29" s="138"/>
+      <c r="J29" s="179"/>
+      <c r="K29" s="179"/>
       <c r="L29" s="26"/>
       <c r="N29" s="7"/>
     </row>
@@ -4422,8 +5088,8 @@
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" s="25"/>
-      <c r="J30" s="139"/>
-      <c r="K30" s="139"/>
+      <c r="J30" s="180"/>
+      <c r="K30" s="180"/>
       <c r="L30" s="100"/>
       <c r="N30" s="7"/>
     </row>
@@ -5799,6 +6465,36 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Organizacion xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">ENEL</Organizacion>
+    <Tipo_x0020_Auditoria xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">Contraprestación ENEL</Tipo_x0020_Auditoria>
+    <TaxCatchAll xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">
+      <Value>24</Value>
+      <Value>48</Value>
+    </TaxCatchAll>
+    <mc2ce51dacb94f6bb557174edb7a5e78 xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2023</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">46694912-6763-4975-9fd9-c77e0dec2cab</TermId>
+        </TermInfo>
+      </Terms>
+    </mc2ce51dacb94f6bb557174edb7a5e78>
+    <o8e2700eeee4411fa2022dc950eab810 xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Agosto</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8293fe82-d099-439f-94cb-06d5159728f8</TermId>
+        </TermInfo>
+      </Terms>
+    </o8e2700eeee4411fa2022dc950eab810>
+    <Auditoría xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">Documentos Mensuales ENEL</Auditoría>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Proceso" ma:contentTypeID="0x010100D161328C4CF32444B4DE139121D8DE5300467F84FB5DF4654FA6987AFE6EF80A25" ma:contentTypeVersion="12" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9bb515c4dce2649fb18d4a58e4a0061d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f" xmlns:ns3="ef91d8dc-f46d-44cd-a575-8661b4cef94d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="661945d0f72ea79a21c93577ebd50501" ns2:_="" ns3:_="">
     <xsd:import namespace="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f"/>
@@ -6032,36 +6728,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Organizacion xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">ENEL</Organizacion>
-    <Tipo_x0020_Auditoria xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">Contraprestación ENEL</Tipo_x0020_Auditoria>
-    <TaxCatchAll xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">
-      <Value>24</Value>
-      <Value>48</Value>
-    </TaxCatchAll>
-    <mc2ce51dacb94f6bb557174edb7a5e78 xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2023</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">46694912-6763-4975-9fd9-c77e0dec2cab</TermId>
-        </TermInfo>
-      </Terms>
-    </mc2ce51dacb94f6bb557174edb7a5e78>
-    <o8e2700eeee4411fa2022dc950eab810 xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Agosto</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8293fe82-d099-439f-94cb-06d5159728f8</TermId>
-        </TermInfo>
-      </Terms>
-    </o8e2700eeee4411fa2022dc950eab810>
-    <Auditoría xmlns="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f">Documentos Mensuales ENEL</Auditoría>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E5FBB0-2BF7-47BA-93B4-8BCCB17B4A48}">
   <ds:schemaRefs>
@@ -6071,6 +6737,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2122C46F-BE4A-408F-90D1-8534F571971D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef91d8dc-f46d-44cd-a575-8661b4cef94d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E55A0763-6430-4A4D-B6B1-15B4D947EEFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6089,23 +6772,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2122C46F-BE4A-408F-90D1-8534F571971D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5bd77e89-8cc9-469c-8406-c2d9f8eb3a4f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ef91d8dc-f46d-44cd-a575-8661b4cef94d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{65bb3aad-376d-42f5-83f9-9beaea39fdc4}" enabled="0" method="" siteId="{65bb3aad-376d-42f5-83f9-9beaea39fdc4}" removed="1"/>

</xml_diff>

<commit_message>
Observaciones del Reprote FacturaCPGNA Fee
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/CalculoFacturaCpgnaConFee50.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/CalculoFacturaCpgnaConFee50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27816"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F9FF3C-0615-4AAF-9307-F0C1AD1E746E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B6F883-F064-4647-BFFD-12250B073416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="701" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fact CPGNA" sheetId="2" r:id="rId1"/>
@@ -51,22 +51,11 @@
     <definedName name="TipoCambio_Items">'Fact CPGNA'!$I$9:$J$10</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="202">
   <si>
     <r>
       <t xml:space="preserve">A) Determinación del </t>
@@ -718,9 +707,6 @@
     <t>{{PrecioFacturacion}}</t>
   </si>
   <si>
-    <t>{{Cm}}</t>
-  </si>
-  <si>
     <t>{{VolumenProcesamientoGna}}</t>
   </si>
   <si>
@@ -871,6 +857,15 @@
   </si>
   <si>
     <t>{{item.Glp}}</t>
+  </si>
+  <si>
+    <t>{{Cm}}  %</t>
+  </si>
+  <si>
+    <t>{{Cm}} %</t>
+  </si>
+  <si>
+    <t>{{Pref}}</t>
   </si>
 </sst>
 </file>
@@ -2336,7 +2331,7 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2531,44 +2526,43 @@
     <xf numFmtId="171" fontId="64" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2577,37 +2571,31 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="16" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2619,10 +2607,7 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2672,18 +2657,17 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="357" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="47" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2714,17 +2698,14 @@
     <xf numFmtId="0" fontId="73" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="358">
@@ -3125,11 +3106,11 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>259080</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3708,45 +3689,45 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:R99"/>
+  <dimension ref="C2:R99"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="145" zoomScaleNormal="85" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="145" zoomScaleNormal="85" zoomScaleSheetLayoutView="145" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:18">
       <c r="N2" s="90"/>
     </row>
     <row r="3" spans="3:18">
-      <c r="C3" s="171" t="s">
+      <c r="C3" s="166" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
       <c r="N3" s="88"/>
     </row>
     <row r="4" spans="3:18">
-      <c r="C4" s="171"/>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
       <c r="N4" s="89"/>
     </row>
     <row r="5" spans="3:18">
@@ -3770,26 +3751,26 @@
     </row>
     <row r="8" spans="3:18" ht="12.75" customHeight="1">
       <c r="G8" s="91"/>
-      <c r="I8" s="172" t="s">
+      <c r="I8" s="167" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="173"/>
+      <c r="J8" s="168"/>
       <c r="M8" s="82"/>
       <c r="N8" s="7"/>
       <c r="O8" s="83"/>
     </row>
     <row r="9" spans="3:18" ht="13.5" customHeight="1">
-      <c r="C9" s="170" t="s">
+      <c r="C9" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="170"/>
+      <c r="D9" s="165"/>
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="71"/>
       <c r="H9" s="71"/>
-      <c r="I9" s="133" t="s">
+      <c r="I9" s="130" t="s">
         <v>141</v>
       </c>
       <c r="J9" s="106" t="s">
@@ -3825,16 +3806,16 @@
       <c r="R10" s="63"/>
     </row>
     <row r="11" spans="3:18" ht="13.5" customHeight="1">
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="128" t="s">
+      <c r="D11" s="125" t="s">
         <v>138</v>
       </c>
-      <c r="E11" s="126" t="s">
+      <c r="E11" s="123" t="s">
         <v>139</v>
       </c>
-      <c r="F11" s="127" t="s">
+      <c r="F11" s="124" t="s">
         <v>140</v>
       </c>
       <c r="G11" s="71">
@@ -3856,8 +3837,8 @@
       <c r="F12" s="87"/>
       <c r="G12" s="91"/>
       <c r="H12" s="71"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="132"/>
+      <c r="I12" s="128"/>
+      <c r="J12" s="129"/>
       <c r="K12" s="54"/>
       <c r="M12" s="82"/>
       <c r="N12" s="7"/>
@@ -3871,10 +3852,10 @@
       <c r="F13" s="87"/>
       <c r="G13" s="91"/>
       <c r="H13" s="71"/>
-      <c r="I13" s="110" t="s">
+      <c r="I13" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="111" t="s">
+      <c r="J13" s="110" t="s">
         <v>136</v>
       </c>
       <c r="K13" s="54"/>
@@ -3889,8 +3870,8 @@
       <c r="E14" s="86"/>
       <c r="F14" s="87"/>
       <c r="G14" s="91"/>
-      <c r="I14" s="129"/>
-      <c r="J14" s="130"/>
+      <c r="I14" s="126"/>
+      <c r="J14" s="127"/>
       <c r="K14" s="54"/>
       <c r="M14" s="82"/>
       <c r="N14" s="7"/>
@@ -3902,15 +3883,15 @@
         <v>8</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="125" t="s">
+      <c r="E15" s="122" t="s">
         <v>143</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="91"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="130"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="127"/>
       <c r="K15" s="54"/>
       <c r="M15" s="82"/>
       <c r="N15" s="7"/>
@@ -3919,8 +3900,8 @@
     </row>
     <row r="16" spans="3:18" ht="13.5" customHeight="1">
       <c r="E16" s="1"/>
-      <c r="I16" s="129"/>
-      <c r="J16" s="130"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="127"/>
       <c r="K16" s="54"/>
       <c r="M16" s="82"/>
       <c r="N16" s="7"/>
@@ -3937,8 +3918,8 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="129"/>
-      <c r="J17" s="130"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="127"/>
       <c r="K17" s="54"/>
       <c r="M17" s="82"/>
       <c r="N17" s="7"/>
@@ -3958,8 +3939,8 @@
       <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="129"/>
-      <c r="J18" s="130"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="127"/>
       <c r="K18" s="54"/>
       <c r="M18" s="82"/>
       <c r="N18" s="7"/>
@@ -3976,8 +3957,8 @@
       <c r="F19" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="129"/>
-      <c r="J19" s="130"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="127"/>
       <c r="K19" s="54"/>
       <c r="M19" s="82"/>
       <c r="N19" s="7"/>
@@ -3986,8 +3967,8 @@
     </row>
     <row r="20" spans="3:18" ht="13.5" customHeight="1" thickBot="1">
       <c r="E20" s="1"/>
-      <c r="I20" s="129"/>
-      <c r="J20" s="130"/>
+      <c r="I20" s="126"/>
+      <c r="J20" s="127"/>
       <c r="K20" s="54"/>
       <c r="M20" s="82"/>
       <c r="N20" s="7"/>
@@ -4005,8 +3986,8 @@
       <c r="F21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="129"/>
-      <c r="J21" s="130"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="127"/>
       <c r="K21" s="54"/>
       <c r="M21" s="82"/>
       <c r="N21" s="7"/>
@@ -4018,8 +3999,8 @@
       <c r="D22" s="3"/>
       <c r="E22" s="51"/>
       <c r="F22" s="3"/>
-      <c r="I22" s="129"/>
-      <c r="J22" s="130"/>
+      <c r="I22" s="126"/>
+      <c r="J22" s="127"/>
       <c r="K22" s="54"/>
       <c r="M22" s="82"/>
       <c r="N22" s="7"/>
@@ -4031,8 +4012,8 @@
       <c r="D23" s="3"/>
       <c r="E23" s="51"/>
       <c r="F23" s="3"/>
-      <c r="I23" s="129"/>
-      <c r="J23" s="130"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="127"/>
       <c r="K23" s="54"/>
       <c r="M23" s="82"/>
       <c r="N23" s="7"/>
@@ -4044,8 +4025,8 @@
       <c r="D24" s="3"/>
       <c r="E24" s="51"/>
       <c r="F24" s="3"/>
-      <c r="I24" s="129"/>
-      <c r="J24" s="130"/>
+      <c r="I24" s="126"/>
+      <c r="J24" s="127"/>
       <c r="K24" s="54"/>
       <c r="M24" s="82"/>
       <c r="N24" s="7"/>
@@ -4057,8 +4038,8 @@
       <c r="D25" s="3"/>
       <c r="E25" s="51"/>
       <c r="F25" s="3"/>
-      <c r="I25" s="129"/>
-      <c r="J25" s="130"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="127"/>
       <c r="K25" s="54"/>
       <c r="M25" s="82"/>
       <c r="N25" s="7"/>
@@ -4070,8 +4051,8 @@
       <c r="D26" s="3"/>
       <c r="E26" s="51"/>
       <c r="F26" s="3"/>
-      <c r="I26" s="129"/>
-      <c r="J26" s="130"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="127"/>
       <c r="K26" s="54"/>
       <c r="M26" s="82"/>
       <c r="N26" s="7"/>
@@ -4083,8 +4064,8 @@
       <c r="D27" s="3"/>
       <c r="E27" s="51"/>
       <c r="F27" s="3"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="130"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="127"/>
       <c r="K27" s="54"/>
       <c r="M27" s="82"/>
       <c r="N27" s="7"/>
@@ -4096,8 +4077,8 @@
       <c r="D28" s="3"/>
       <c r="E28" s="51"/>
       <c r="F28" s="3"/>
-      <c r="I28" s="129"/>
-      <c r="J28" s="130"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="127"/>
       <c r="K28" s="54"/>
       <c r="M28" s="82"/>
       <c r="N28" s="7"/>
@@ -4122,7 +4103,7 @@
       <c r="Q30" s="55"/>
       <c r="R30" s="55"/>
     </row>
-    <row r="31" spans="3:18" ht="14.25">
+    <row r="31" spans="3:18" ht="13.8">
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
@@ -4134,42 +4115,42 @@
       <c r="R31" s="55"/>
     </row>
     <row r="32" spans="3:18">
-      <c r="C32" s="174" t="s">
-        <v>161</v>
-      </c>
-      <c r="D32" s="174"/>
-      <c r="E32" s="174"/>
-      <c r="F32" s="174"/>
-      <c r="G32" s="174"/>
-      <c r="H32" s="174"/>
-      <c r="I32" s="135"/>
-      <c r="J32" s="135"/>
+      <c r="C32" s="169" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="169"/>
+      <c r="E32" s="169"/>
+      <c r="F32" s="169"/>
+      <c r="G32" s="169"/>
+      <c r="H32" s="169"/>
+      <c r="I32" s="131"/>
+      <c r="J32" s="131"/>
       <c r="M32" s="62"/>
       <c r="N32" s="54"/>
       <c r="O32" s="54"/>
       <c r="P32" s="55"/>
     </row>
     <row r="33" spans="3:12">
-      <c r="C33" s="169" t="s">
+      <c r="C33" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="169"/>
+      <c r="D33" s="164"/>
+      <c r="E33" s="164"/>
+      <c r="F33" s="164"/>
+      <c r="G33" s="164"/>
+      <c r="H33" s="164"/>
       <c r="I33" s="84"/>
       <c r="J33" s="84"/>
     </row>
     <row r="34" spans="3:12">
-      <c r="C34" s="169" t="s">
+      <c r="C34" s="164" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="169"/>
-      <c r="E34" s="169"/>
-      <c r="F34" s="169"/>
-      <c r="G34" s="169"/>
-      <c r="H34" s="169"/>
+      <c r="D34" s="164"/>
+      <c r="E34" s="164"/>
+      <c r="F34" s="164"/>
+      <c r="G34" s="164"/>
+      <c r="H34" s="164"/>
       <c r="I34" s="84"/>
       <c r="J34" s="84"/>
     </row>
@@ -4193,9 +4174,8 @@
       <c r="C42" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="122" t="str">
-        <f>+E21</f>
-        <v>{{PrefPeríodo}}</v>
+      <c r="D42" s="119" t="s">
+        <v>201</v>
       </c>
       <c r="E42" t="s">
         <v>26</v>
@@ -4206,8 +4186,8 @@
       <c r="C43" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="124" t="s">
-        <v>160</v>
+      <c r="D43" s="121" t="s">
+        <v>159</v>
       </c>
       <c r="E43" t="s">
         <v>28</v>
@@ -4218,8 +4198,8 @@
       <c r="C44" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="124" t="s">
-        <v>159</v>
+      <c r="D44" s="121" t="s">
+        <v>158</v>
       </c>
       <c r="E44" t="s">
         <v>30</v>
@@ -4229,8 +4209,8 @@
       <c r="C46" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="123" t="s">
-        <v>158</v>
+      <c r="D46" s="120" t="s">
+        <v>157</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>32</v>
@@ -4251,8 +4231,8 @@
       <c r="C51" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="122" t="s">
-        <v>157</v>
+      <c r="D51" s="119" t="s">
+        <v>156</v>
       </c>
       <c r="E51" s="84" t="s">
         <v>32</v>
@@ -4263,7 +4243,7 @@
         <v>36</v>
       </c>
       <c r="G52" s="57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H52" t="s">
         <v>37</v>
@@ -4290,8 +4270,8 @@
       <c r="C56" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D56" s="121" t="s">
-        <v>155</v>
+      <c r="D56" s="163" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="3:14">
@@ -4324,15 +4304,15 @@
       <c r="C64" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="D64" s="120" t="s">
-        <v>155</v>
+      <c r="D64" s="116" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="3:17">
       <c r="C65" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="117" t="s">
+      <c r="D65" s="116" t="s">
         <v>154</v>
       </c>
       <c r="E65" s="84" t="s">
@@ -4343,7 +4323,7 @@
       <c r="C66" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="D66" s="119" t="s">
+      <c r="D66" s="118" t="s">
         <v>153</v>
       </c>
       <c r="E66" s="84" t="s">
@@ -4354,7 +4334,7 @@
       <c r="C67" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D67" s="118" t="s">
+      <c r="D67" s="117" t="s">
         <v>152</v>
       </c>
       <c r="E67" t="s">
@@ -4368,7 +4348,7 @@
         <v>49</v>
       </c>
       <c r="D68" s="20"/>
-      <c r="E68" s="116" t="s">
+      <c r="E68" s="115" t="s">
         <v>151</v>
       </c>
       <c r="F68" s="25" t="s">
@@ -4391,7 +4371,7 @@
         <v>52</v>
       </c>
       <c r="D72" s="73"/>
-      <c r="E72" s="114" t="s">
+      <c r="E72" s="113" t="s">
         <v>150</v>
       </c>
       <c r="F72" s="74" t="s">
@@ -4405,7 +4385,7 @@
         <v>54</v>
       </c>
       <c r="D73" s="3"/>
-      <c r="E73" s="115" t="s">
+      <c r="E73" s="114" t="s">
         <v>149</v>
       </c>
       <c r="F73" s="76" t="s">
@@ -4417,7 +4397,7 @@
         <v>55</v>
       </c>
       <c r="D74" s="78"/>
-      <c r="E74" s="113" t="s">
+      <c r="E74" s="112" t="s">
         <v>148</v>
       </c>
       <c r="F74" s="79" t="s">
@@ -4429,7 +4409,7 @@
         <v>56</v>
       </c>
       <c r="D77" s="73"/>
-      <c r="E77" s="112" t="s">
+      <c r="E77" s="111" t="s">
         <v>147</v>
       </c>
       <c r="F77" s="74" t="s">
@@ -4441,7 +4421,7 @@
         <v>58</v>
       </c>
       <c r="D78" s="3"/>
-      <c r="E78" s="113" t="s">
+      <c r="E78" s="112" t="s">
         <v>146</v>
       </c>
       <c r="F78" s="76" t="s">
@@ -4455,65 +4435,60 @@
       <c r="D79" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="E79" s="113" t="s">
+      <c r="E79" s="112" t="s">
         <v>145</v>
       </c>
       <c r="F79" s="79" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="2:13">
+    <row r="82" spans="3:13">
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="2:13">
+    <row r="83" spans="3:13">
       <c r="E83" s="13"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="2:13">
+    <row r="84" spans="3:13">
       <c r="C84" s="3"/>
       <c r="D84" s="57"/>
       <c r="F84" s="58"/>
       <c r="L84" s="71"/>
       <c r="M84" s="71"/>
     </row>
-    <row r="85" spans="2:13">
+    <row r="85" spans="3:13">
       <c r="C85" s="84"/>
       <c r="L85" s="71"/>
       <c r="M85" s="71"/>
     </row>
-    <row r="86" spans="2:13">
+    <row r="86" spans="3:13">
       <c r="C86" s="84"/>
       <c r="L86" s="71"/>
       <c r="M86" s="71"/>
     </row>
-    <row r="87" spans="2:13">
+    <row r="87" spans="3:13">
       <c r="C87" s="59"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="2:13">
+    <row r="88" spans="3:13">
       <c r="C88" s="59"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="2:13">
+    <row r="89" spans="3:13">
       <c r="C89" s="59"/>
       <c r="D89" s="60"/>
     </row>
-    <row r="90" spans="2:13">
+    <row r="90" spans="3:13">
       <c r="D90" s="53"/>
     </row>
-    <row r="91" spans="2:13">
+    <row r="91" spans="3:13">
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="2:13">
-      <c r="B92" s="107"/>
-      <c r="C92" s="109"/>
-      <c r="D92" s="108"/>
-      <c r="E92" s="107"/>
-    </row>
-    <row r="93" spans="2:13">
-      <c r="C93" s="107"/>
-    </row>
-    <row r="96" spans="2:13">
+    <row r="92" spans="3:13">
+      <c r="C92" s="108"/>
+      <c r="D92" s="107"/>
+    </row>
+    <row r="96" spans="3:13">
       <c r="H96" s="84"/>
     </row>
     <row r="97" spans="3:8">
@@ -4544,7 +4519,7 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="1.0236220472440944" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -4558,11 +4533,11 @@
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>36</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>60960</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:colOff>259080</xdr:colOff>
                 <xdr:row>40</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -4582,15 +4557,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C20844-8914-4D92-B039-BDC0FF141079}">
   <dimension ref="B2:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="2" spans="2:18">
       <c r="C2" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -4599,267 +4574,266 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="2:18" ht="15.75">
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="M3" s="137"/>
+    <row r="3" spans="2:18" ht="15.6">
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="M3" s="133"/>
     </row>
     <row r="4" spans="2:18">
-      <c r="N4" s="134" t="s">
+      <c r="N4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="134"/>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="C6" s="171"/>
+      <c r="D6" s="171"/>
+      <c r="E6" s="135" t="s">
         <v>164</v>
       </c>
-      <c r="O4" s="138"/>
-    </row>
-    <row r="6" spans="2:18">
-      <c r="C6" s="176"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="139" t="s">
+      <c r="F6" s="172" t="s">
         <v>165</v>
       </c>
-      <c r="F6" s="177" t="s">
+      <c r="G6" s="173"/>
+      <c r="H6" s="136" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="G6" s="178"/>
-      <c r="H6" s="140" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" s="140" t="s">
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
+      <c r="M6" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="141"/>
-      <c r="K6" s="141"/>
-      <c r="M6" s="142" t="s">
+      <c r="O6" s="136" t="s">
         <v>168</v>
       </c>
-      <c r="O6" s="140" t="s">
+      <c r="P6" s="136" t="s">
         <v>169</v>
       </c>
-      <c r="P6" s="140" t="s">
+      <c r="Q6" s="136" t="s">
         <v>170</v>
       </c>
-      <c r="Q6" s="140" t="s">
+    </row>
+    <row r="7" spans="2:18" ht="21">
+      <c r="B7" s="136" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" ht="22.5">
-      <c r="B7" s="140" t="s">
+      <c r="C7" s="139" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="D7" s="136" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="136" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="140" t="s">
+      <c r="F7" s="136" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="140" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="136" t="s">
+        <v>176</v>
+      </c>
+      <c r="I7" s="136" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="136" t="s">
         <v>171</v>
       </c>
-      <c r="E7" s="140" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="140" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="144" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="140" t="s">
+      <c r="M7" s="141" t="s">
         <v>177</v>
       </c>
-      <c r="I7" s="140" t="s">
+      <c r="N7" s="137"/>
+      <c r="O7" s="136" t="s">
         <v>177</v>
       </c>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
-      <c r="L7" s="140" t="s">
-        <v>172</v>
-      </c>
-      <c r="M7" s="145" t="s">
+      <c r="P7" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q7" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="142" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="143" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="144" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="144" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="145" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="145" t="s">
+        <v>189</v>
+      </c>
+      <c r="H8" s="144" t="s">
+        <v>190</v>
+      </c>
+      <c r="I8" s="146" t="s">
+        <v>191</v>
+      </c>
+      <c r="J8" s="137"/>
+      <c r="K8" s="137"/>
+      <c r="L8" s="142" t="s">
+        <v>184</v>
+      </c>
+      <c r="M8" s="145" t="s">
+        <v>186</v>
+      </c>
+      <c r="N8" s="13"/>
+      <c r="O8" s="145" t="s">
+        <v>198</v>
+      </c>
+      <c r="P8" s="145" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q8" s="145" t="s">
+        <v>186</v>
+      </c>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="142"/>
+      <c r="C9" s="143"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="137"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="145"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="147"/>
+      <c r="P9" s="147"/>
+      <c r="Q9" s="147"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="L10" s="149"/>
+      <c r="M10" s="150"/>
+      <c r="N10" s="148"/>
+      <c r="O10" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="P10" s="151" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q10" s="151" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="149"/>
+      <c r="D11" s="150" t="s">
         <v>178</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="140" t="s">
-        <v>178</v>
-      </c>
-      <c r="P7" s="140" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q7" s="140" t="s">
-        <v>178</v>
-      </c>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="2:18">
-      <c r="B8" s="146" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" s="147" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" s="148" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="148" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" s="149" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="149" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="148" t="s">
-        <v>191</v>
-      </c>
-      <c r="I8" s="150" t="s">
+      <c r="H11" s="119" t="s">
         <v>192</v>
       </c>
-      <c r="J8" s="141"/>
-      <c r="K8" s="141"/>
-      <c r="L8" s="146" t="s">
-        <v>185</v>
-      </c>
-      <c r="M8" s="149" t="s">
-        <v>187</v>
-      </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="149" t="s">
-        <v>199</v>
-      </c>
-      <c r="P8" s="149" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q8" s="149" t="s">
-        <v>187</v>
-      </c>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" spans="2:18">
-      <c r="B9" s="146"/>
-      <c r="C9" s="165"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="149"/>
-      <c r="G9" s="166"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="150"/>
-      <c r="J9" s="141"/>
-      <c r="K9" s="141"/>
-      <c r="L9" s="146"/>
-      <c r="M9" s="149"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="151"/>
-      <c r="P9" s="151"/>
-      <c r="Q9" s="151"/>
-    </row>
-    <row r="10" spans="2:18">
-      <c r="L10" s="153"/>
-      <c r="M10" s="154"/>
-      <c r="N10" s="152"/>
-      <c r="O10" s="155" t="s">
-        <v>197</v>
-      </c>
-      <c r="P10" s="155" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q10" s="155" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18">
-      <c r="B11" s="153"/>
-      <c r="D11" s="154" t="s">
+      <c r="I11" t="s">
         <v>179</v>
       </c>
-      <c r="H11" s="167" t="s">
+      <c r="L11" s="149"/>
+      <c r="M11" s="150"/>
+      <c r="N11" s="148"/>
+      <c r="O11" s="150"/>
+      <c r="P11" s="150"/>
+      <c r="Q11" s="150"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="149"/>
+      <c r="C12" s="150"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
+      <c r="F12" s="150"/>
+      <c r="G12" s="150"/>
+      <c r="H12" s="150"/>
+      <c r="L12" s="152" t="s">
+        <v>180</v>
+      </c>
+      <c r="M12" s="150"/>
+      <c r="N12" s="148"/>
+      <c r="O12" s="150"/>
+      <c r="Q12" s="150"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="C13" s="150"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="153"/>
+      <c r="F13" s="153"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="161" t="s">
         <v>193</v>
       </c>
-      <c r="I11" t="s">
-        <v>180</v>
-      </c>
-      <c r="L11" s="153"/>
-      <c r="M11" s="154"/>
-      <c r="N11" s="152"/>
-      <c r="O11" s="154"/>
-      <c r="P11" s="154"/>
-      <c r="Q11" s="154"/>
-    </row>
-    <row r="12" spans="2:18">
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="154"/>
-      <c r="F12" s="154"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="154"/>
-      <c r="L12" s="156" t="s">
+      <c r="I13" s="155" t="s">
         <v>181</v>
       </c>
-      <c r="M12" s="154"/>
-      <c r="N12" s="152"/>
-      <c r="O12" s="154"/>
-      <c r="Q12" s="154"/>
-    </row>
-    <row r="13" spans="2:18">
-      <c r="C13" s="154"/>
-      <c r="D13" s="158"/>
-      <c r="E13" s="157"/>
-      <c r="F13" s="157"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="168" t="s">
-        <v>194</v>
-      </c>
-      <c r="I13" s="159" t="s">
+      <c r="M13" s="150"/>
+      <c r="N13" s="148"/>
+      <c r="O13" s="150"/>
+      <c r="P13" s="156"/>
+      <c r="Q13" s="150"/>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="159"/>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="C22" s="170" t="s">
         <v>182</v>
       </c>
-      <c r="M13" s="154"/>
-      <c r="N13" s="152"/>
-      <c r="O13" s="154"/>
-      <c r="P13" s="160"/>
-      <c r="Q13" s="154"/>
-    </row>
-    <row r="21" spans="2:17">
-      <c r="C21" s="107"/>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161"/>
-      <c r="J21" s="163"/>
-    </row>
-    <row r="22" spans="2:17">
-      <c r="C22" s="175" t="s">
+      <c r="D22" s="170"/>
+      <c r="E22" s="170"/>
+      <c r="G22" s="170" t="s">
         <v>183</v>
       </c>
-      <c r="D22" s="175"/>
-      <c r="E22" s="175"/>
-      <c r="G22" s="175" t="s">
-        <v>184</v>
-      </c>
-      <c r="H22" s="175"/>
-      <c r="I22" s="175"/>
-      <c r="J22" s="164"/>
-      <c r="K22" s="182"/>
-      <c r="L22" s="181" t="s">
+      <c r="H22" s="170"/>
+      <c r="I22" s="170"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="162"/>
+      <c r="L22" s="174" t="s">
+        <v>182</v>
+      </c>
+      <c r="M22" s="170"/>
+      <c r="O22" s="170" t="s">
         <v>183</v>
       </c>
-      <c r="M22" s="175"/>
-      <c r="O22" s="175" t="s">
-        <v>184</v>
-      </c>
-      <c r="P22" s="175"/>
-      <c r="Q22" s="175"/>
+      <c r="P22" s="170"/>
+      <c r="Q22" s="170"/>
     </row>
     <row r="24" spans="2:17">
-      <c r="B24" s="162"/>
+      <c r="B24" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4887,21 +4861,21 @@
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="21" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="21" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:11" ht="9" customHeight="1"/>
@@ -4940,10 +4914,10 @@
     </row>
     <row r="16" spans="4:11" ht="25.5" customHeight="1"/>
     <row r="17" spans="5:15" ht="27" customHeight="1">
-      <c r="J17" s="179" t="s">
+      <c r="J17" s="175" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="179"/>
+      <c r="K17" s="175"/>
       <c r="L17" s="24" t="s">
         <v>68</v>
       </c>
@@ -4967,11 +4941,11 @@
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="180" t="str">
+      <c r="J19" s="176" t="str">
         <f>+'Fact CPGNA'!E68</f>
         <v>{{CmPrecioPsec}}</v>
       </c>
-      <c r="K19" s="180"/>
+      <c r="K19" s="176"/>
       <c r="L19" s="99" t="e">
         <f>ROUND(+E19*J19,2)</f>
         <v>#VALUE!</v>
@@ -4993,8 +4967,8 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="180"/>
-      <c r="K21" s="180"/>
+      <c r="J21" s="176"/>
+      <c r="K21" s="176"/>
       <c r="L21" s="99"/>
     </row>
     <row r="22" spans="5:15">
@@ -5077,8 +5051,8 @@
       <c r="G29" s="34"/>
       <c r="H29" s="35"/>
       <c r="I29" s="36"/>
-      <c r="J29" s="179"/>
-      <c r="K29" s="179"/>
+      <c r="J29" s="175"/>
+      <c r="K29" s="175"/>
       <c r="L29" s="26"/>
       <c r="N29" s="7"/>
     </row>
@@ -5088,8 +5062,8 @@
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" s="25"/>
-      <c r="J30" s="180"/>
-      <c r="K30" s="180"/>
+      <c r="J30" s="176"/>
+      <c r="K30" s="176"/>
       <c r="L30" s="100"/>
       <c r="N30" s="7"/>
     </row>
@@ -5247,7 +5221,7 @@
     <row r="55" spans="3:21">
       <c r="K55" s="39"/>
     </row>
-    <row r="56" spans="3:21" ht="15.75">
+    <row r="56" spans="3:21" ht="15.6">
       <c r="K56" s="39"/>
       <c r="N56" s="43"/>
       <c r="O56" s="44" t="s">

</xml_diff>